<commit_message>
Updated timesheet for j2
</commit_message>
<xml_diff>
--- a/Timesheet-evaluation.xlsx
+++ b/Timesheet-evaluation.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="105">
   <si>
     <t xml:space="preserve">ETU001844</t>
   </si>
@@ -258,6 +258,75 @@
   </si>
   <si>
     <t xml:space="preserve">Model VcoureurCategorie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">create_v_temps_coureur_etape_equipe_coureur_categorie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">create_v_classement_categorie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">create_v_classement_categories</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Model ClassementCategorie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Model ClassementCategorieEquipe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">classement par categorie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Admin modules</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Import etapes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Import resultat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Import Points</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Page d’import</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Page Import Point</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kilometrage sur les componsant joueur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kilometrage sur les model joueur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Integration </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Module Admin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Generer categorie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Admin Schema</t>
+  </si>
+  <si>
+    <t xml:space="preserve">generate_categorie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ETU001845</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ETU001846</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Generere categorie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ETU001847</t>
   </si>
   <si>
     <t xml:space="preserve">*Valeur en Minutes</t>
@@ -277,7 +346,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00\ %"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -314,6 +383,12 @@
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="3">
@@ -371,7 +446,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -410,6 +485,18 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -499,8 +586,8 @@
   </sheetPr>
   <dimension ref="A1:H1003"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A29" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A95" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A102" activeCellId="0" sqref="A102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.22265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2148,7 +2235,7 @@
       <c r="A65" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="B65" s="7" t="s">
+      <c r="B65" s="8" t="s">
         <v>72</v>
       </c>
       <c r="C65" s="7" t="s">
@@ -2354,60 +2441,816 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A73" s="7"/>
-      <c r="B73" s="8"/>
-      <c r="C73" s="7"/>
-      <c r="D73" s="7"/>
-      <c r="E73" s="7" t="n">
-        <f aca="false">SUM(E4:E64)</f>
-        <v>198</v>
-      </c>
-      <c r="F73" s="7" t="n">
-        <f aca="false">SUM(F4:F64)</f>
-        <v>172</v>
-      </c>
+    <row r="73" customFormat="false" ht="40.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A73" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B73" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="C73" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D73" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="E73" s="10" t="n">
+        <v>5</v>
+      </c>
+      <c r="F73" s="10"/>
       <c r="G73" s="7" t="n">
-        <f aca="false">SUM(G4:G64)</f>
-        <v>79</v>
-      </c>
-      <c r="H73" s="10" t="n">
+        <f aca="false">E73-F73</f>
+        <v>5</v>
+      </c>
+      <c r="H73" s="9" t="n">
         <f aca="false">(F73/(F73+G73))</f>
-        <v>0.685258964143426</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="93" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="95" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="103" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="28.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A74" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B74" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C74" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D74" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E74" s="7" t="n">
+        <v>5</v>
+      </c>
+      <c r="F74" s="7"/>
+      <c r="G74" s="7" t="n">
+        <f aca="false">E74-F74</f>
+        <v>5</v>
+      </c>
+      <c r="H74" s="9" t="n">
+        <f aca="false">(F74/(F74+G74))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="31.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A75" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B75" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C75" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D75" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="E75" s="7" t="n">
+        <v>5</v>
+      </c>
+      <c r="F75" s="7"/>
+      <c r="G75" s="7" t="n">
+        <f aca="false">E75-F75</f>
+        <v>5</v>
+      </c>
+      <c r="H75" s="9" t="n">
+        <f aca="false">(F75/(F75+G75))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="30.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A76" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B76" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C76" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D76" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E76" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="F76" s="7"/>
+      <c r="G76" s="7" t="n">
+        <f aca="false">E76-F76</f>
+        <v>3</v>
+      </c>
+      <c r="H76" s="9" t="n">
+        <f aca="false">(F76/(F76+G76))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="40" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A77" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B77" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="C77" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D77" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="E77" s="10" t="n">
+        <v>3</v>
+      </c>
+      <c r="F77" s="10"/>
+      <c r="G77" s="7" t="n">
+        <f aca="false">E77-F77</f>
+        <v>3</v>
+      </c>
+      <c r="H77" s="9" t="n">
+        <f aca="false">(F77/(F77+G77))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A78" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B78" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C78" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D78" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E78" s="7" t="n">
+        <v>4</v>
+      </c>
+      <c r="F78" s="7"/>
+      <c r="G78" s="7" t="n">
+        <f aca="false">E78-F78</f>
+        <v>4</v>
+      </c>
+      <c r="H78" s="9" t="n">
+        <f aca="false">(F78/(F78+G78))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A79" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B79" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C79" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D79" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="E79" s="7" t="n">
+        <v>4</v>
+      </c>
+      <c r="F79" s="7"/>
+      <c r="G79" s="7" t="n">
+        <f aca="false">E79-F79</f>
+        <v>4</v>
+      </c>
+      <c r="H79" s="9" t="n">
+        <f aca="false">(F79/(F79+G79))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A80" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="B80" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C80" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D80" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E80" s="10" t="n">
+        <v>3</v>
+      </c>
+      <c r="F80" s="10"/>
+      <c r="G80" s="7" t="n">
+        <f aca="false">E80-F80</f>
+        <v>3</v>
+      </c>
+      <c r="H80" s="9" t="n">
+        <f aca="false">(F80/(F80+G80))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A81" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B81" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C81" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D81" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="E81" s="7" t="n">
+        <v>5</v>
+      </c>
+      <c r="F81" s="7"/>
+      <c r="G81" s="7" t="n">
+        <f aca="false">E81-F81</f>
+        <v>5</v>
+      </c>
+      <c r="H81" s="9" t="n">
+        <f aca="false">(F81/(F81+G81))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A82" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B82" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C82" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D82" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E82" s="7" t="n">
+        <v>10</v>
+      </c>
+      <c r="F82" s="7"/>
+      <c r="G82" s="7" t="n">
+        <f aca="false">E82-F82</f>
+        <v>10</v>
+      </c>
+      <c r="H82" s="9" t="n">
+        <f aca="false">(F82/(F82+G82))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A83" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B83" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C83" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D83" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="E83" s="7" t="n">
+        <v>5</v>
+      </c>
+      <c r="F83" s="7"/>
+      <c r="G83" s="7" t="n">
+        <f aca="false">E83-F83</f>
+        <v>5</v>
+      </c>
+      <c r="H83" s="9" t="n">
+        <f aca="false">(F83/(F83+G83))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A84" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B84" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="C84" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D84" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E84" s="10" t="n">
+        <v>5</v>
+      </c>
+      <c r="F84" s="10"/>
+      <c r="G84" s="7" t="n">
+        <f aca="false">E84-F84</f>
+        <v>5</v>
+      </c>
+      <c r="H84" s="9" t="n">
+        <f aca="false">(F84/(F84+G84))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A85" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B85" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C85" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D85" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="E85" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="F85" s="7"/>
+      <c r="G85" s="7" t="n">
+        <f aca="false">E85-F85</f>
+        <v>3</v>
+      </c>
+      <c r="H85" s="9" t="n">
+        <f aca="false">(F85/(F85+G85))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A86" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B86" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C86" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D86" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E86" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="F86" s="7"/>
+      <c r="G86" s="7" t="n">
+        <f aca="false">E86-F86</f>
+        <v>3</v>
+      </c>
+      <c r="H86" s="9" t="n">
+        <f aca="false">(F86/(F86+G86))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A87" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B87" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C87" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D87" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="E87" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="F87" s="7"/>
+      <c r="G87" s="7" t="n">
+        <f aca="false">E87-F87</f>
+        <v>3</v>
+      </c>
+      <c r="H87" s="9" t="n">
+        <f aca="false">(F87/(F87+G87))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A88" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B88" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C88" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D88" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E88" s="7" t="n">
+        <v>5</v>
+      </c>
+      <c r="F88" s="7"/>
+      <c r="G88" s="7" t="n">
+        <f aca="false">E88-F88</f>
+        <v>5</v>
+      </c>
+      <c r="H88" s="9" t="n">
+        <f aca="false">(F88/(F88+G88))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A89" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B89" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C89" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D89" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="E89" s="7" t="n">
+        <v>5</v>
+      </c>
+      <c r="F89" s="7"/>
+      <c r="G89" s="7" t="n">
+        <f aca="false">E89-F89</f>
+        <v>5</v>
+      </c>
+      <c r="H89" s="9" t="n">
+        <f aca="false">(F89/(F89+G89))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A90" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B90" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C90" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D90" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E90" s="10" t="n">
+        <v>5</v>
+      </c>
+      <c r="F90" s="10"/>
+      <c r="G90" s="7" t="n">
+        <f aca="false">E90-F90</f>
+        <v>5</v>
+      </c>
+      <c r="H90" s="9" t="n">
+        <f aca="false">(F90/(F90+G90))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A91" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B91" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C91" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D91" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="E91" s="7" t="n">
+        <v>5</v>
+      </c>
+      <c r="F91" s="7"/>
+      <c r="G91" s="7" t="n">
+        <f aca="false">E91-F91</f>
+        <v>5</v>
+      </c>
+      <c r="H91" s="9" t="n">
+        <f aca="false">(F91/(F91+G91))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A92" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B92" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C92" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D92" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E92" s="7" t="n">
+        <v>5</v>
+      </c>
+      <c r="F92" s="7"/>
+      <c r="G92" s="7" t="n">
+        <f aca="false">E92-F92</f>
+        <v>5</v>
+      </c>
+      <c r="H92" s="9" t="n">
+        <f aca="false">(F92/(F92+G92))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A93" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B93" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C93" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D93" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="E93" s="7" t="n">
+        <v>5</v>
+      </c>
+      <c r="F93" s="7"/>
+      <c r="G93" s="7" t="n">
+        <f aca="false">E93-F93</f>
+        <v>5</v>
+      </c>
+      <c r="H93" s="9" t="n">
+        <f aca="false">(F93/(F93+G93))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A94" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B94" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C94" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D94" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E94" s="7" t="n">
+        <v>5</v>
+      </c>
+      <c r="F94" s="7"/>
+      <c r="G94" s="7" t="n">
+        <f aca="false">E94-F94</f>
+        <v>5</v>
+      </c>
+      <c r="H94" s="9" t="n">
+        <f aca="false">(F94/(F94+G94))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="30.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A95" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B95" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="C95" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D95" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="E95" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="F95" s="7"/>
+      <c r="G95" s="7" t="n">
+        <f aca="false">E95-F95</f>
+        <v>3</v>
+      </c>
+      <c r="H95" s="9" t="n">
+        <f aca="false">(F95/(F95+G95))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="26.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A96" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B96" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="C96" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D96" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E96" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="F96" s="7"/>
+      <c r="G96" s="7" t="n">
+        <f aca="false">E96-F96</f>
+        <v>2</v>
+      </c>
+      <c r="H96" s="9" t="n">
+        <f aca="false">(F96/(F96+G96))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="29.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A97" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B97" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="C97" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D97" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="E97" s="7" t="n">
+        <v>5</v>
+      </c>
+      <c r="F97" s="7"/>
+      <c r="G97" s="7" t="n">
+        <f aca="false">E97-F97</f>
+        <v>5</v>
+      </c>
+      <c r="H97" s="9" t="n">
+        <f aca="false">(F97/(F97+G97))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A98" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="B98" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C98" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="D98" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E98" s="10" t="n">
+        <v>4</v>
+      </c>
+      <c r="F98" s="10"/>
+      <c r="G98" s="7" t="n">
+        <f aca="false">E98-F98</f>
+        <v>4</v>
+      </c>
+      <c r="H98" s="9" t="n">
+        <f aca="false">(F98/(F98+G98))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A99" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B99" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="C99" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D99" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="E99" s="7" t="n">
+        <v>10</v>
+      </c>
+      <c r="F99" s="7"/>
+      <c r="G99" s="7" t="n">
+        <f aca="false">E99-F99</f>
+        <v>10</v>
+      </c>
+      <c r="H99" s="9" t="n">
+        <f aca="false">(F99/(F99+G99))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A100" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D100" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="E100" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F100" s="0"/>
+      <c r="G100" s="7" t="n">
+        <f aca="false">E100-F100</f>
+        <v>2</v>
+      </c>
+      <c r="H100" s="9" t="n">
+        <f aca="false">(F100/(F100+G100))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A101" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D101" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="E101" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G101" s="7" t="n">
+        <f aca="false">E101-F101</f>
+        <v>2</v>
+      </c>
+      <c r="H101" s="9" t="n">
+        <f aca="false">(F101/(F101+G101))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A102" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D102" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="E102" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="G102" s="7" t="n">
+        <f aca="false">E102-F102</f>
+        <v>5</v>
+      </c>
+      <c r="H102" s="9" t="n">
+        <f aca="false">(F102/(F102+G102))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A103" s="0"/>
+      <c r="B103" s="0"/>
+      <c r="C103" s="0"/>
+      <c r="H103" s="9" t="e">
+        <f aca="false">(F103/(F103+G103))</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
     <row r="104" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="105" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="105" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A105" s="7"/>
+      <c r="B105" s="8"/>
+      <c r="C105" s="7"/>
+      <c r="D105" s="7"/>
+      <c r="E105" s="7" t="n">
+        <f aca="false">SUM(E4:E104)</f>
+        <v>363</v>
+      </c>
+      <c r="F105" s="7" t="n">
+        <f aca="false">SUM(F4:F104)</f>
+        <v>203</v>
+      </c>
+      <c r="G105" s="7" t="n">
+        <f aca="false">SUM(G4:G104)</f>
+        <v>227</v>
+      </c>
+      <c r="H105" s="13" t="n">
+        <f aca="false">(F105/(F105+G105))</f>
+        <v>0.472093023255814</v>
+      </c>
+    </row>
     <row r="106" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="107" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="108" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -3332,39 +4175,39 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>79</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="11" t="s">
-        <v>80</v>
+      <c r="A2" s="14" t="s">
+        <v>103</v>
       </c>
       <c r="B2" s="3" t="n">
-        <f aca="false">Feuil1!E73</f>
-        <v>198</v>
+        <f aca="false">Feuil1!E105</f>
+        <v>363</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="14" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="3" t="n">
-        <f aca="false">Feuil1!F73</f>
-        <v>172</v>
+        <f aca="false">Feuil1!F105</f>
+        <v>203</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="14" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="3" t="n">
-        <f aca="false">Feuil1!G73</f>
-        <v>79</v>
+        <f aca="false">Feuil1!G105</f>
+        <v>227</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="3" t="s">
-        <v>81</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>